<commit_message>
Deploying to gh-pages from  @ 63f96d68f082b13f3f0b694e23b8c57a3a3845a8 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/5.4.1.xlsx
+++ b/en/downloads/data-excel/5.4.1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
   <si>
     <t>5.4.1 Жынысы, курагы жана жашаган жери боюнча үйдү жыйноо жана үй ишин кылуу боюнча төлөнбөгөн эмгекке карата убакыттын үлүшү</t>
   </si>
@@ -77,6 +77,42 @@
   </si>
   <si>
     <t>Items</t>
+  </si>
+  <si>
+    <t>Шаар жерлери</t>
+  </si>
+  <si>
+    <t>Городские поселения</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Айыл аймагы</t>
+  </si>
+  <si>
+    <t>Сельская местность</t>
+  </si>
+  <si>
+    <t>Village</t>
+  </si>
+  <si>
+    <t>Эркектер</t>
+  </si>
+  <si>
+    <t>Мужчины</t>
+  </si>
+  <si>
+    <t>Man</t>
+  </si>
+  <si>
+    <t>Аялдар</t>
+  </si>
+  <si>
+    <t>Женщины</t>
+  </si>
+  <si>
+    <t>Woman</t>
   </si>
 </sst>
 </file>
@@ -86,7 +122,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +160,13 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -154,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -175,6 +218,24 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -481,11 +542,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
@@ -540,70 +599,342 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="8">
         <v>13.2</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="8">
         <v>11.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3">
-        <v>1.7</v>
+        <v>12.5</v>
       </c>
       <c r="E6" s="3">
-        <v>2.6</v>
+        <v>10.7</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="3">
+        <v>13.9</v>
+      </c>
+      <c r="E7" s="3">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="E8" s="3">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="3">
+        <v>18.8</v>
+      </c>
+      <c r="E9" s="3">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1.7</v>
+      </c>
+      <c r="E10" s="8">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="E13" s="3">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B15" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D15" s="8">
         <v>0.9</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E15" s="11">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="E16" s="7">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="E17" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="E18" s="7">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="E19" s="7">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B20" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C20" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D20" s="12">
         <v>0.5</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E20" s="12">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0.4</v>
+      </c>
+      <c r="E21" s="13">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="13">
+        <v>0.6</v>
+      </c>
+      <c r="E22" s="13">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="13">
+        <v>0.6</v>
+      </c>
+      <c r="E23" s="13">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="E24" s="5">
         <v>0.3</v>
       </c>
     </row>

</xml_diff>